<commit_message>
added the training and inference pipeline for 5 day forecast
</commit_message>
<xml_diff>
--- a/artifacts/data_preprocessing/Lstm_data_preprocessed.xlsx
+++ b/artifacts/data_preprocessing/Lstm_data_preprocessed.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1829"/>
+  <dimension ref="A1:B1994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
         <v>43620</v>
       </c>
       <c r="B6" t="n">
-        <v>83.33333333333333</v>
+        <v>83.33333333333334</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         <v>43621</v>
       </c>
       <c r="B7" t="n">
-        <v>82.66666666666667</v>
+        <v>82.66666666666666</v>
       </c>
     </row>
     <row r="8">
@@ -526,7 +526,7 @@
         <v>43625</v>
       </c>
       <c r="B11" t="n">
-        <v>80.86666666666666</v>
+        <v>80.86666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -630,7 +630,7 @@
         <v>43638</v>
       </c>
       <c r="B24" t="n">
-        <v>79.13333333333334</v>
+        <v>79.13333333333333</v>
       </c>
     </row>
     <row r="25">
@@ -742,7 +742,7 @@
         <v>43652</v>
       </c>
       <c r="B38" t="n">
-        <v>78.86666666666666</v>
+        <v>78.86666666666667</v>
       </c>
     </row>
     <row r="39">
@@ -1038,7 +1038,7 @@
         <v>43689</v>
       </c>
       <c r="B75" t="n">
-        <v>81.55000000000001</v>
+        <v>81.55</v>
       </c>
     </row>
     <row r="76">
@@ -1086,7 +1086,7 @@
         <v>43695</v>
       </c>
       <c r="B81" t="n">
-        <v>82.39999999999999</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="82">
@@ -1246,7 +1246,7 @@
         <v>43715</v>
       </c>
       <c r="B101" t="n">
-        <v>84.93333333333332</v>
+        <v>84.93333333333334</v>
       </c>
     </row>
     <row r="102">
@@ -1278,7 +1278,7 @@
         <v>43719</v>
       </c>
       <c r="B105" t="n">
-        <v>86.69999999999999</v>
+        <v>86.7</v>
       </c>
     </row>
     <row r="106">
@@ -1358,7 +1358,7 @@
         <v>43729</v>
       </c>
       <c r="B115" t="n">
-        <v>87.46666666666667</v>
+        <v>87.46666666666665</v>
       </c>
     </row>
     <row r="116">
@@ -1366,7 +1366,7 @@
         <v>43730</v>
       </c>
       <c r="B116" t="n">
-        <v>87.53333333333333</v>
+        <v>87.53333333333335</v>
       </c>
     </row>
     <row r="117">
@@ -1422,7 +1422,7 @@
         <v>43737</v>
       </c>
       <c r="B123" t="n">
-        <v>88.39999999999999</v>
+        <v>88.40000000000001</v>
       </c>
     </row>
     <row r="124">
@@ -1694,7 +1694,7 @@
         <v>43771</v>
       </c>
       <c r="B157" t="n">
-        <v>92.33333333333333</v>
+        <v>92.33333333333334</v>
       </c>
     </row>
     <row r="158">
@@ -1702,7 +1702,7 @@
         <v>43772</v>
       </c>
       <c r="B158" t="n">
-        <v>92.46666666666667</v>
+        <v>92.46666666666665</v>
       </c>
     </row>
     <row r="159">
@@ -1806,7 +1806,7 @@
         <v>43785</v>
       </c>
       <c r="B171" t="n">
-        <v>93.46666666666667</v>
+        <v>93.46666666666665</v>
       </c>
     </row>
     <row r="172">
@@ -1814,7 +1814,7 @@
         <v>43786</v>
       </c>
       <c r="B172" t="n">
-        <v>93.13333333333333</v>
+        <v>93.13333333333334</v>
       </c>
     </row>
     <row r="173">
@@ -1862,7 +1862,7 @@
         <v>43792</v>
       </c>
       <c r="B178" t="n">
-        <v>95.53333333333333</v>
+        <v>95.53333333333335</v>
       </c>
     </row>
     <row r="179">
@@ -2206,7 +2206,7 @@
         <v>43835</v>
       </c>
       <c r="B221" t="n">
-        <v>95.66666666666667</v>
+        <v>95.66666666666666</v>
       </c>
     </row>
     <row r="222">
@@ -2254,7 +2254,7 @@
         <v>43841</v>
       </c>
       <c r="B227" t="n">
-        <v>96.33330000000001</v>
+        <v>96.33329999999999</v>
       </c>
     </row>
     <row r="228">
@@ -2262,7 +2262,7 @@
         <v>43842</v>
       </c>
       <c r="B228" t="n">
-        <v>96.49995</v>
+        <v>96.49994999999998</v>
       </c>
     </row>
     <row r="229">
@@ -2310,7 +2310,7 @@
         <v>43848</v>
       </c>
       <c r="B234" t="n">
-        <v>94.46666666666667</v>
+        <v>94.46666666666665</v>
       </c>
     </row>
     <row r="235">
@@ -2374,7 +2374,7 @@
         <v>43856</v>
       </c>
       <c r="B242" t="n">
-        <v>92.46666666666667</v>
+        <v>92.46666666666665</v>
       </c>
     </row>
     <row r="243">
@@ -2486,7 +2486,7 @@
         <v>43870</v>
       </c>
       <c r="B256" t="n">
-        <v>90.53333333333333</v>
+        <v>90.53333333333335</v>
       </c>
     </row>
     <row r="257">
@@ -2534,7 +2534,7 @@
         <v>43876</v>
       </c>
       <c r="B262" t="n">
-        <v>91.46666666666667</v>
+        <v>91.46666666666665</v>
       </c>
     </row>
     <row r="263">
@@ -2542,7 +2542,7 @@
         <v>43877</v>
       </c>
       <c r="B263" t="n">
-        <v>91.33333333333333</v>
+        <v>91.33333333333334</v>
       </c>
     </row>
     <row r="264">
@@ -2646,7 +2646,7 @@
         <v>43890</v>
       </c>
       <c r="B276" t="n">
-        <v>91.53333333333333</v>
+        <v>91.53333333333335</v>
       </c>
     </row>
     <row r="277">
@@ -2654,7 +2654,7 @@
         <v>43891</v>
       </c>
       <c r="B277" t="n">
-        <v>91.66666666666667</v>
+        <v>91.66666666666666</v>
       </c>
     </row>
     <row r="278">
@@ -2798,7 +2798,7 @@
         <v>43909</v>
       </c>
       <c r="B295" t="n">
-        <v>91.62978723404255</v>
+        <v>91.62978723404257</v>
       </c>
     </row>
     <row r="296">
@@ -2814,7 +2814,7 @@
         <v>43911</v>
       </c>
       <c r="B297" t="n">
-        <v>91.70638297872341</v>
+        <v>91.7063829787234</v>
       </c>
     </row>
     <row r="298">
@@ -2822,7 +2822,7 @@
         <v>43912</v>
       </c>
       <c r="B298" t="n">
-        <v>91.74468085106383</v>
+        <v>91.74468085106382</v>
       </c>
     </row>
     <row r="299">
@@ -2838,7 +2838,7 @@
         <v>43914</v>
       </c>
       <c r="B300" t="n">
-        <v>91.82127659574469</v>
+        <v>91.82127659574468</v>
       </c>
     </row>
     <row r="301">
@@ -2846,7 +2846,7 @@
         <v>43915</v>
       </c>
       <c r="B301" t="n">
-        <v>91.85957446808511</v>
+        <v>91.8595744680851</v>
       </c>
     </row>
     <row r="302">
@@ -2854,7 +2854,7 @@
         <v>43916</v>
       </c>
       <c r="B302" t="n">
-        <v>91.89787234042554</v>
+        <v>91.89787234042552</v>
       </c>
     </row>
     <row r="303">
@@ -2870,7 +2870,7 @@
         <v>43918</v>
       </c>
       <c r="B304" t="n">
-        <v>91.97446808510639</v>
+        <v>91.97446808510638</v>
       </c>
     </row>
     <row r="305">
@@ -2878,7 +2878,7 @@
         <v>43919</v>
       </c>
       <c r="B305" t="n">
-        <v>92.01276595744682</v>
+        <v>92.0127659574468</v>
       </c>
     </row>
     <row r="306">
@@ -2934,7 +2934,7 @@
         <v>43926</v>
       </c>
       <c r="B312" t="n">
-        <v>92.28085106382979</v>
+        <v>92.2808510638298</v>
       </c>
     </row>
     <row r="313">
@@ -2942,7 +2942,7 @@
         <v>43927</v>
       </c>
       <c r="B313" t="n">
-        <v>92.31914893617022</v>
+        <v>92.31914893617021</v>
       </c>
     </row>
     <row r="314">
@@ -2950,7 +2950,7 @@
         <v>43928</v>
       </c>
       <c r="B314" t="n">
-        <v>92.35744680851064</v>
+        <v>92.35744680851063</v>
       </c>
     </row>
     <row r="315">
@@ -2958,7 +2958,7 @@
         <v>43929</v>
       </c>
       <c r="B315" t="n">
-        <v>92.39574468085107</v>
+        <v>92.39574468085105</v>
       </c>
     </row>
     <row r="316">
@@ -2974,7 +2974,7 @@
         <v>43931</v>
       </c>
       <c r="B317" t="n">
-        <v>92.47234042553193</v>
+        <v>92.47234042553191</v>
       </c>
     </row>
     <row r="318">
@@ -2982,7 +2982,7 @@
         <v>43932</v>
       </c>
       <c r="B318" t="n">
-        <v>92.51063829787235</v>
+        <v>92.51063829787233</v>
       </c>
     </row>
     <row r="319">
@@ -3038,7 +3038,7 @@
         <v>43939</v>
       </c>
       <c r="B325" t="n">
-        <v>92.77872340425532</v>
+        <v>92.77872340425533</v>
       </c>
     </row>
     <row r="326">
@@ -3062,7 +3062,7 @@
         <v>43942</v>
       </c>
       <c r="B328" t="n">
-        <v>92.8936170212766</v>
+        <v>92.89361702127661</v>
       </c>
     </row>
     <row r="329">
@@ -3078,7 +3078,7 @@
         <v>43944</v>
       </c>
       <c r="B330" t="n">
-        <v>92.97021276595746</v>
+        <v>92.97021276595744</v>
       </c>
     </row>
     <row r="331">
@@ -3086,7 +3086,7 @@
         <v>43945</v>
       </c>
       <c r="B331" t="n">
-        <v>93.00851063829788</v>
+        <v>93.00851063829786</v>
       </c>
     </row>
     <row r="332">
@@ -3110,7 +3110,7 @@
         <v>43948</v>
       </c>
       <c r="B334" t="n">
-        <v>93.12340425531916</v>
+        <v>93.12340425531914</v>
       </c>
     </row>
     <row r="335">
@@ -3118,7 +3118,7 @@
         <v>43949</v>
       </c>
       <c r="B335" t="n">
-        <v>93.16170212765958</v>
+        <v>93.16170212765957</v>
       </c>
     </row>
     <row r="336">
@@ -3174,7 +3174,7 @@
         <v>43956</v>
       </c>
       <c r="B342" t="n">
-        <v>93.42978723404255</v>
+        <v>93.42978723404256</v>
       </c>
     </row>
     <row r="343">
@@ -3198,7 +3198,7 @@
         <v>43959</v>
       </c>
       <c r="B345" t="n">
-        <v>93.54468085106383</v>
+        <v>93.54468085106382</v>
       </c>
     </row>
     <row r="346">
@@ -3214,7 +3214,7 @@
         <v>43961</v>
       </c>
       <c r="B347" t="n">
-        <v>93.62127659574469</v>
+        <v>93.62127659574467</v>
       </c>
     </row>
     <row r="348">
@@ -3222,7 +3222,7 @@
         <v>43962</v>
       </c>
       <c r="B348" t="n">
-        <v>93.65957446808511</v>
+        <v>93.6595744680851</v>
       </c>
     </row>
     <row r="349">
@@ -3278,7 +3278,7 @@
         <v>43969</v>
       </c>
       <c r="B355" t="n">
-        <v>93.92765957446808</v>
+        <v>93.92765957446809</v>
       </c>
     </row>
     <row r="356">
@@ -3302,7 +3302,7 @@
         <v>43972</v>
       </c>
       <c r="B358" t="n">
-        <v>94.04255319148936</v>
+        <v>94.04255319148938</v>
       </c>
     </row>
     <row r="359">
@@ -3310,7 +3310,7 @@
         <v>43973</v>
       </c>
       <c r="B359" t="n">
-        <v>94.08085106382978</v>
+        <v>94.0808510638298</v>
       </c>
     </row>
     <row r="360">
@@ -3318,7 +3318,7 @@
         <v>43974</v>
       </c>
       <c r="B360" t="n">
-        <v>94.11914893617022</v>
+        <v>94.11914893617021</v>
       </c>
     </row>
     <row r="361">
@@ -3326,7 +3326,7 @@
         <v>43975</v>
       </c>
       <c r="B361" t="n">
-        <v>94.15744680851064</v>
+        <v>94.15744680851063</v>
       </c>
     </row>
     <row r="362">
@@ -3350,7 +3350,7 @@
         <v>43978</v>
       </c>
       <c r="B364" t="n">
-        <v>94.27234042553192</v>
+        <v>94.27234042553191</v>
       </c>
     </row>
     <row r="365">
@@ -3414,7 +3414,7 @@
         <v>43986</v>
       </c>
       <c r="B372" t="n">
-        <v>94.57872340425531</v>
+        <v>94.57872340425533</v>
       </c>
     </row>
     <row r="373">
@@ -3438,7 +3438,7 @@
         <v>43989</v>
       </c>
       <c r="B375" t="n">
-        <v>94.69361702127659</v>
+        <v>94.69361702127661</v>
       </c>
     </row>
     <row r="376">
@@ -3454,7 +3454,7 @@
         <v>43991</v>
       </c>
       <c r="B377" t="n">
-        <v>94.77021276595745</v>
+        <v>94.77021276595744</v>
       </c>
     </row>
     <row r="378">
@@ -3462,7 +3462,7 @@
         <v>43992</v>
       </c>
       <c r="B378" t="n">
-        <v>94.80851063829788</v>
+        <v>94.80851063829786</v>
       </c>
     </row>
     <row r="379">
@@ -3486,7 +3486,7 @@
         <v>43995</v>
       </c>
       <c r="B381" t="n">
-        <v>94.92340425531916</v>
+        <v>94.92340425531914</v>
       </c>
     </row>
     <row r="382">
@@ -3758,7 +3758,7 @@
         <v>44029</v>
       </c>
       <c r="B415" t="n">
-        <v>92.8</v>
+        <v>92.59999999999999</v>
       </c>
     </row>
     <row r="416">
@@ -3766,7 +3766,7 @@
         <v>44030</v>
       </c>
       <c r="B416" t="n">
-        <v>92.8</v>
+        <v>92.65000000000001</v>
       </c>
     </row>
     <row r="417">
@@ -3774,7 +3774,7 @@
         <v>44031</v>
       </c>
       <c r="B417" t="n">
-        <v>92.8</v>
+        <v>92.7</v>
       </c>
     </row>
     <row r="418">
@@ -3782,7 +3782,7 @@
         <v>44032</v>
       </c>
       <c r="B418" t="n">
-        <v>92.8</v>
+        <v>92.75</v>
       </c>
     </row>
     <row r="419">
@@ -3822,7 +3822,7 @@
         <v>44037</v>
       </c>
       <c r="B423" t="n">
-        <v>92.33333333333333</v>
+        <v>92.33333333333334</v>
       </c>
     </row>
     <row r="424">
@@ -3830,7 +3830,7 @@
         <v>44038</v>
       </c>
       <c r="B424" t="n">
-        <v>92.46666666666667</v>
+        <v>92.46666666666665</v>
       </c>
     </row>
     <row r="425">
@@ -3910,7 +3910,7 @@
         <v>44048</v>
       </c>
       <c r="B434" t="n">
-        <v>92.69999999999999</v>
+        <v>92.7</v>
       </c>
     </row>
     <row r="435">
@@ -3934,7 +3934,7 @@
         <v>44051</v>
       </c>
       <c r="B437" t="n">
-        <v>92.53333333333333</v>
+        <v>92.53333333333335</v>
       </c>
     </row>
     <row r="438">
@@ -3942,7 +3942,7 @@
         <v>44052</v>
       </c>
       <c r="B438" t="n">
-        <v>92.66666666666667</v>
+        <v>92.66666666666666</v>
       </c>
     </row>
     <row r="439">
@@ -3998,7 +3998,7 @@
         <v>44059</v>
       </c>
       <c r="B445" t="n">
-        <v>91.60000000000001</v>
+        <v>91.59999999999999</v>
       </c>
     </row>
     <row r="446">
@@ -4046,7 +4046,7 @@
         <v>44065</v>
       </c>
       <c r="B451" t="n">
-        <v>91.46666666666667</v>
+        <v>91.46666666666665</v>
       </c>
     </row>
     <row r="452">
@@ -4054,7 +4054,7 @@
         <v>44066</v>
       </c>
       <c r="B452" t="n">
-        <v>91.53333333333333</v>
+        <v>91.53333333333335</v>
       </c>
     </row>
     <row r="453">
@@ -4270,7 +4270,7 @@
         <v>44093</v>
       </c>
       <c r="B479" t="n">
-        <v>92.46666666666667</v>
+        <v>92.46666666666665</v>
       </c>
     </row>
     <row r="480">
@@ -4278,7 +4278,7 @@
         <v>44094</v>
       </c>
       <c r="B480" t="n">
-        <v>92.53333333333333</v>
+        <v>92.53333333333335</v>
       </c>
     </row>
     <row r="481">
@@ -4382,7 +4382,7 @@
         <v>44107</v>
       </c>
       <c r="B493" t="n">
-        <v>93.39999999999999</v>
+        <v>93.40000000000001</v>
       </c>
     </row>
     <row r="494">
@@ -4446,7 +4446,7 @@
         <v>44115</v>
       </c>
       <c r="B501" t="n">
-        <v>95.33333333333333</v>
+        <v>95.33333333333334</v>
       </c>
     </row>
     <row r="502">
@@ -4494,7 +4494,7 @@
         <v>44121</v>
       </c>
       <c r="B507" t="n">
-        <v>95.46666666666667</v>
+        <v>95.46666666666665</v>
       </c>
     </row>
     <row r="508">
@@ -4502,7 +4502,7 @@
         <v>44122</v>
       </c>
       <c r="B508" t="n">
-        <v>95.53333333333333</v>
+        <v>95.53333333333335</v>
       </c>
     </row>
     <row r="509">
@@ -4550,7 +4550,7 @@
         <v>44128</v>
       </c>
       <c r="B514" t="n">
-        <v>97.28641975308642</v>
+        <v>97.04000000000001</v>
       </c>
     </row>
     <row r="515">
@@ -4558,7 +4558,7 @@
         <v>44129</v>
       </c>
       <c r="B515" t="n">
-        <v>97.37283950617284</v>
+        <v>96.88</v>
       </c>
     </row>
     <row r="516">
@@ -4566,7 +4566,7 @@
         <v>44130</v>
       </c>
       <c r="B516" t="n">
-        <v>97.45925925925926</v>
+        <v>96.72</v>
       </c>
     </row>
     <row r="517">
@@ -4574,7 +4574,7 @@
         <v>44131</v>
       </c>
       <c r="B517" t="n">
-        <v>97.54567901234569</v>
+        <v>96.56</v>
       </c>
     </row>
     <row r="518">
@@ -4582,7 +4582,7 @@
         <v>44132</v>
       </c>
       <c r="B518" t="n">
-        <v>97.6320987654321</v>
+        <v>96.40000000000001</v>
       </c>
     </row>
     <row r="519">
@@ -4590,7 +4590,7 @@
         <v>44133</v>
       </c>
       <c r="B519" t="n">
-        <v>97.71851851851852</v>
+        <v>96.23999999999999</v>
       </c>
     </row>
     <row r="520">
@@ -4598,7 +4598,7 @@
         <v>44134</v>
       </c>
       <c r="B520" t="n">
-        <v>97.80493827160494</v>
+        <v>96.08</v>
       </c>
     </row>
     <row r="521">
@@ -4606,7 +4606,7 @@
         <v>44135</v>
       </c>
       <c r="B521" t="n">
-        <v>97.89135802469136</v>
+        <v>95.92</v>
       </c>
     </row>
     <row r="522">
@@ -4614,7 +4614,7 @@
         <v>44136</v>
       </c>
       <c r="B522" t="n">
-        <v>97.97777777777777</v>
+        <v>95.76000000000001</v>
       </c>
     </row>
     <row r="523">
@@ -4622,7 +4622,7 @@
         <v>44137</v>
       </c>
       <c r="B523" t="n">
-        <v>98.06419753086421</v>
+        <v>95.59999999999999</v>
       </c>
     </row>
     <row r="524">
@@ -4630,7 +4630,7 @@
         <v>44138</v>
       </c>
       <c r="B524" t="n">
-        <v>98.15061728395062</v>
+        <v>95.44</v>
       </c>
     </row>
     <row r="525">
@@ -4638,7 +4638,7 @@
         <v>44139</v>
       </c>
       <c r="B525" t="n">
-        <v>98.23703703703704</v>
+        <v>95.28</v>
       </c>
     </row>
     <row r="526">
@@ -4646,7 +4646,7 @@
         <v>44140</v>
       </c>
       <c r="B526" t="n">
-        <v>98.32345679012346</v>
+        <v>95.12</v>
       </c>
     </row>
     <row r="527">
@@ -4654,7 +4654,7 @@
         <v>44141</v>
       </c>
       <c r="B527" t="n">
-        <v>98.40987654320988</v>
+        <v>94.95999999999999</v>
       </c>
     </row>
     <row r="528">
@@ -4662,7 +4662,7 @@
         <v>44142</v>
       </c>
       <c r="B528" t="n">
-        <v>98.49629629629629</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="529">
@@ -4670,7 +4670,7 @@
         <v>44143</v>
       </c>
       <c r="B529" t="n">
-        <v>98.58271604938273</v>
+        <v>94.64</v>
       </c>
     </row>
     <row r="530">
@@ -4678,7 +4678,7 @@
         <v>44144</v>
       </c>
       <c r="B530" t="n">
-        <v>98.66913580246914</v>
+        <v>94.48</v>
       </c>
     </row>
     <row r="531">
@@ -4686,7 +4686,7 @@
         <v>44145</v>
       </c>
       <c r="B531" t="n">
-        <v>98.75555555555556</v>
+        <v>94.31999999999999</v>
       </c>
     </row>
     <row r="532">
@@ -4694,7 +4694,7 @@
         <v>44146</v>
       </c>
       <c r="B532" t="n">
-        <v>98.84197530864198</v>
+        <v>94.16</v>
       </c>
     </row>
     <row r="533">
@@ -4702,7 +4702,7 @@
         <v>44147</v>
       </c>
       <c r="B533" t="n">
-        <v>98.92839506172839</v>
+        <v>94</v>
       </c>
     </row>
     <row r="534">
@@ -4710,7 +4710,7 @@
         <v>44148</v>
       </c>
       <c r="B534" t="n">
-        <v>99.01481481481481</v>
+        <v>94</v>
       </c>
     </row>
     <row r="535">
@@ -4718,7 +4718,7 @@
         <v>44149</v>
       </c>
       <c r="B535" t="n">
-        <v>99.10123456790124</v>
+        <v>94.17</v>
       </c>
     </row>
     <row r="536">
@@ -4726,7 +4726,7 @@
         <v>44150</v>
       </c>
       <c r="B536" t="n">
-        <v>99.18765432098766</v>
+        <v>94.34</v>
       </c>
     </row>
     <row r="537">
@@ -4734,7 +4734,7 @@
         <v>44151</v>
       </c>
       <c r="B537" t="n">
-        <v>99.27407407407408</v>
+        <v>94.51000000000001</v>
       </c>
     </row>
     <row r="538">
@@ -4742,7 +4742,7 @@
         <v>44152</v>
       </c>
       <c r="B538" t="n">
-        <v>99.3604938271605</v>
+        <v>94.68000000000001</v>
       </c>
     </row>
     <row r="539">
@@ -4750,7 +4750,7 @@
         <v>44153</v>
       </c>
       <c r="B539" t="n">
-        <v>99.44691358024691</v>
+        <v>94.84999999999999</v>
       </c>
     </row>
     <row r="540">
@@ -4758,7 +4758,7 @@
         <v>44154</v>
       </c>
       <c r="B540" t="n">
-        <v>99.53333333333333</v>
+        <v>95.02</v>
       </c>
     </row>
     <row r="541">
@@ -4766,7 +4766,7 @@
         <v>44155</v>
       </c>
       <c r="B541" t="n">
-        <v>99.61975308641976</v>
+        <v>95.19</v>
       </c>
     </row>
     <row r="542">
@@ -4774,7 +4774,7 @@
         <v>44156</v>
       </c>
       <c r="B542" t="n">
-        <v>99.70617283950618</v>
+        <v>95.36</v>
       </c>
     </row>
     <row r="543">
@@ -4782,7 +4782,7 @@
         <v>44157</v>
       </c>
       <c r="B543" t="n">
-        <v>99.7925925925926</v>
+        <v>95.53</v>
       </c>
     </row>
     <row r="544">
@@ -4790,7 +4790,7 @@
         <v>44158</v>
       </c>
       <c r="B544" t="n">
-        <v>99.87901234567902</v>
+        <v>95.7</v>
       </c>
     </row>
     <row r="545">
@@ -4798,7 +4798,7 @@
         <v>44159</v>
       </c>
       <c r="B545" t="n">
-        <v>99.96543209876543</v>
+        <v>95.87</v>
       </c>
     </row>
     <row r="546">
@@ -4806,7 +4806,7 @@
         <v>44160</v>
       </c>
       <c r="B546" t="n">
-        <v>100.0518518518519</v>
+        <v>96.04000000000001</v>
       </c>
     </row>
     <row r="547">
@@ -4814,7 +4814,7 @@
         <v>44161</v>
       </c>
       <c r="B547" t="n">
-        <v>100.1382716049383</v>
+        <v>96.20999999999999</v>
       </c>
     </row>
     <row r="548">
@@ -4822,7 +4822,7 @@
         <v>44162</v>
       </c>
       <c r="B548" t="n">
-        <v>100.2246913580247</v>
+        <v>96.38</v>
       </c>
     </row>
     <row r="549">
@@ -4830,7 +4830,7 @@
         <v>44163</v>
       </c>
       <c r="B549" t="n">
-        <v>100.3111111111111</v>
+        <v>96.55</v>
       </c>
     </row>
     <row r="550">
@@ -4838,7 +4838,7 @@
         <v>44164</v>
       </c>
       <c r="B550" t="n">
-        <v>100.3975308641975</v>
+        <v>96.72</v>
       </c>
     </row>
     <row r="551">
@@ -4846,7 +4846,7 @@
         <v>44165</v>
       </c>
       <c r="B551" t="n">
-        <v>100.483950617284</v>
+        <v>96.89</v>
       </c>
     </row>
     <row r="552">
@@ -4854,7 +4854,7 @@
         <v>44166</v>
       </c>
       <c r="B552" t="n">
-        <v>100.5703703703704</v>
+        <v>97.06</v>
       </c>
     </row>
     <row r="553">
@@ -4862,7 +4862,7 @@
         <v>44167</v>
       </c>
       <c r="B553" t="n">
-        <v>100.6567901234568</v>
+        <v>97.23</v>
       </c>
     </row>
     <row r="554">
@@ -4870,7 +4870,7 @@
         <v>44168</v>
       </c>
       <c r="B554" t="n">
-        <v>100.7432098765432</v>
+        <v>97.40000000000001</v>
       </c>
     </row>
     <row r="555">
@@ -4878,7 +4878,7 @@
         <v>44169</v>
       </c>
       <c r="B555" t="n">
-        <v>100.8296296296296</v>
+        <v>97.56999999999999</v>
       </c>
     </row>
     <row r="556">
@@ -4886,7 +4886,7 @@
         <v>44170</v>
       </c>
       <c r="B556" t="n">
-        <v>100.9160493827161</v>
+        <v>97.73999999999999</v>
       </c>
     </row>
     <row r="557">
@@ -4894,7 +4894,7 @@
         <v>44171</v>
       </c>
       <c r="B557" t="n">
-        <v>101.0024691358025</v>
+        <v>97.91</v>
       </c>
     </row>
     <row r="558">
@@ -4902,7 +4902,7 @@
         <v>44172</v>
       </c>
       <c r="B558" t="n">
-        <v>101.0888888888889</v>
+        <v>98.08</v>
       </c>
     </row>
     <row r="559">
@@ -4910,7 +4910,7 @@
         <v>44173</v>
       </c>
       <c r="B559" t="n">
-        <v>101.1753086419753</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="560">
@@ -4918,7 +4918,7 @@
         <v>44174</v>
       </c>
       <c r="B560" t="n">
-        <v>101.2617283950617</v>
+        <v>98.42</v>
       </c>
     </row>
     <row r="561">
@@ -4926,7 +4926,7 @@
         <v>44175</v>
       </c>
       <c r="B561" t="n">
-        <v>101.3481481481482</v>
+        <v>98.59</v>
       </c>
     </row>
     <row r="562">
@@ -4934,7 +4934,7 @@
         <v>44176</v>
       </c>
       <c r="B562" t="n">
-        <v>101.4345679012346</v>
+        <v>98.76000000000001</v>
       </c>
     </row>
     <row r="563">
@@ -4942,7 +4942,7 @@
         <v>44177</v>
       </c>
       <c r="B563" t="n">
-        <v>101.520987654321</v>
+        <v>98.93000000000001</v>
       </c>
     </row>
     <row r="564">
@@ -4950,7 +4950,7 @@
         <v>44178</v>
       </c>
       <c r="B564" t="n">
-        <v>101.6074074074074</v>
+        <v>99.09999999999999</v>
       </c>
     </row>
     <row r="565">
@@ -4958,7 +4958,7 @@
         <v>44179</v>
       </c>
       <c r="B565" t="n">
-        <v>101.6938271604938</v>
+        <v>99.27</v>
       </c>
     </row>
     <row r="566">
@@ -4966,7 +4966,7 @@
         <v>44180</v>
       </c>
       <c r="B566" t="n">
-        <v>101.7802469135802</v>
+        <v>99.44</v>
       </c>
     </row>
     <row r="567">
@@ -4974,7 +4974,7 @@
         <v>44181</v>
       </c>
       <c r="B567" t="n">
-        <v>101.8666666666667</v>
+        <v>99.61</v>
       </c>
     </row>
     <row r="568">
@@ -4982,7 +4982,7 @@
         <v>44182</v>
       </c>
       <c r="B568" t="n">
-        <v>101.9530864197531</v>
+        <v>99.78</v>
       </c>
     </row>
     <row r="569">
@@ -4990,7 +4990,7 @@
         <v>44183</v>
       </c>
       <c r="B569" t="n">
-        <v>102.0395061728395</v>
+        <v>99.95</v>
       </c>
     </row>
     <row r="570">
@@ -4998,7 +4998,7 @@
         <v>44184</v>
       </c>
       <c r="B570" t="n">
-        <v>102.1259259259259</v>
+        <v>100.12</v>
       </c>
     </row>
     <row r="571">
@@ -5006,7 +5006,7 @@
         <v>44185</v>
       </c>
       <c r="B571" t="n">
-        <v>102.2123456790123</v>
+        <v>100.29</v>
       </c>
     </row>
     <row r="572">
@@ -5014,7 +5014,7 @@
         <v>44186</v>
       </c>
       <c r="B572" t="n">
-        <v>102.2987654320988</v>
+        <v>100.46</v>
       </c>
     </row>
     <row r="573">
@@ -5022,7 +5022,7 @@
         <v>44187</v>
       </c>
       <c r="B573" t="n">
-        <v>102.3851851851852</v>
+        <v>100.63</v>
       </c>
     </row>
     <row r="574">
@@ -5030,7 +5030,7 @@
         <v>44188</v>
       </c>
       <c r="B574" t="n">
-        <v>102.4716049382716</v>
+        <v>100.8</v>
       </c>
     </row>
     <row r="575">
@@ -5038,7 +5038,7 @@
         <v>44189</v>
       </c>
       <c r="B575" t="n">
-        <v>102.558024691358</v>
+        <v>100.97</v>
       </c>
     </row>
     <row r="576">
@@ -5046,7 +5046,7 @@
         <v>44190</v>
       </c>
       <c r="B576" t="n">
-        <v>102.6444444444444</v>
+        <v>101.14</v>
       </c>
     </row>
     <row r="577">
@@ -5054,7 +5054,7 @@
         <v>44191</v>
       </c>
       <c r="B577" t="n">
-        <v>102.7308641975309</v>
+        <v>101.31</v>
       </c>
     </row>
     <row r="578">
@@ -5062,7 +5062,7 @@
         <v>44192</v>
       </c>
       <c r="B578" t="n">
-        <v>102.8172839506173</v>
+        <v>101.48</v>
       </c>
     </row>
     <row r="579">
@@ -5070,7 +5070,7 @@
         <v>44193</v>
       </c>
       <c r="B579" t="n">
-        <v>102.9037037037037</v>
+        <v>101.65</v>
       </c>
     </row>
     <row r="580">
@@ -5078,7 +5078,7 @@
         <v>44194</v>
       </c>
       <c r="B580" t="n">
-        <v>102.9901234567901</v>
+        <v>101.82</v>
       </c>
     </row>
     <row r="581">
@@ -5086,7 +5086,7 @@
         <v>44195</v>
       </c>
       <c r="B581" t="n">
-        <v>103.0765432098765</v>
+        <v>101.99</v>
       </c>
     </row>
     <row r="582">
@@ -5094,7 +5094,7 @@
         <v>44196</v>
       </c>
       <c r="B582" t="n">
-        <v>103.162962962963</v>
+        <v>102.16</v>
       </c>
     </row>
     <row r="583">
@@ -5102,7 +5102,7 @@
         <v>44197</v>
       </c>
       <c r="B583" t="n">
-        <v>103.2493827160494</v>
+        <v>102.33</v>
       </c>
     </row>
     <row r="584">
@@ -5110,7 +5110,7 @@
         <v>44198</v>
       </c>
       <c r="B584" t="n">
-        <v>103.3358024691358</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="585">
@@ -5118,7 +5118,7 @@
         <v>44199</v>
       </c>
       <c r="B585" t="n">
-        <v>103.4222222222222</v>
+        <v>102.67</v>
       </c>
     </row>
     <row r="586">
@@ -5126,7 +5126,7 @@
         <v>44200</v>
       </c>
       <c r="B586" t="n">
-        <v>103.5086419753086</v>
+        <v>102.84</v>
       </c>
     </row>
     <row r="587">
@@ -5134,7 +5134,7 @@
         <v>44201</v>
       </c>
       <c r="B587" t="n">
-        <v>103.5950617283951</v>
+        <v>103.01</v>
       </c>
     </row>
     <row r="588">
@@ -5142,7 +5142,7 @@
         <v>44202</v>
       </c>
       <c r="B588" t="n">
-        <v>103.6814814814815</v>
+        <v>103.18</v>
       </c>
     </row>
     <row r="589">
@@ -5150,7 +5150,7 @@
         <v>44203</v>
       </c>
       <c r="B589" t="n">
-        <v>103.7679012345679</v>
+        <v>103.35</v>
       </c>
     </row>
     <row r="590">
@@ -5158,7 +5158,7 @@
         <v>44204</v>
       </c>
       <c r="B590" t="n">
-        <v>103.8543209876543</v>
+        <v>103.52</v>
       </c>
     </row>
     <row r="591">
@@ -5166,7 +5166,7 @@
         <v>44205</v>
       </c>
       <c r="B591" t="n">
-        <v>103.9407407407408</v>
+        <v>103.69</v>
       </c>
     </row>
     <row r="592">
@@ -5174,7 +5174,7 @@
         <v>44206</v>
       </c>
       <c r="B592" t="n">
-        <v>104.0271604938272</v>
+        <v>103.86</v>
       </c>
     </row>
     <row r="593">
@@ -5182,7 +5182,7 @@
         <v>44207</v>
       </c>
       <c r="B593" t="n">
-        <v>104.1135802469136</v>
+        <v>104.03</v>
       </c>
     </row>
     <row r="594">
@@ -5342,7 +5342,7 @@
         <v>44227</v>
       </c>
       <c r="B613" t="n">
-        <v>97.53333333333333</v>
+        <v>97.53333333333335</v>
       </c>
     </row>
     <row r="614">
@@ -5398,7 +5398,7 @@
         <v>44234</v>
       </c>
       <c r="B620" t="n">
-        <v>95.53333333333333</v>
+        <v>95.53333333333335</v>
       </c>
     </row>
     <row r="621">
@@ -5550,7 +5550,7 @@
         <v>44253</v>
       </c>
       <c r="B639" t="n">
-        <v>95.94999999999999</v>
+        <v>95.95</v>
       </c>
     </row>
     <row r="640">
@@ -5614,7 +5614,7 @@
         <v>44261</v>
       </c>
       <c r="B647" t="n">
-        <v>96.53333333333333</v>
+        <v>96.53333333333335</v>
       </c>
     </row>
     <row r="648">
@@ -5622,7 +5622,7 @@
         <v>44262</v>
       </c>
       <c r="B648" t="n">
-        <v>96.86666666666667</v>
+        <v>96.86666666666666</v>
       </c>
     </row>
     <row r="649">
@@ -5814,7 +5814,7 @@
         <v>44286</v>
       </c>
       <c r="B672" t="n">
-        <v>99.19999999999999</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="673">
@@ -6286,7 +6286,7 @@
         <v>44345</v>
       </c>
       <c r="B731" t="n">
-        <v>116.5555555555556</v>
+        <v>116.5555555555555</v>
       </c>
     </row>
     <row r="732">
@@ -6382,7 +6382,7 @@
         <v>44357</v>
       </c>
       <c r="B743" t="n">
-        <v>117.3333333333333</v>
+        <v>117.375</v>
       </c>
     </row>
     <row r="744">
@@ -6390,7 +6390,7 @@
         <v>44358</v>
       </c>
       <c r="B744" t="n">
-        <v>117.4666666666667</v>
+        <v>117.55</v>
       </c>
     </row>
     <row r="745">
@@ -6398,7 +6398,7 @@
         <v>44359</v>
       </c>
       <c r="B745" t="n">
-        <v>117.6</v>
+        <v>117.725</v>
       </c>
     </row>
     <row r="746">
@@ -6406,7 +6406,7 @@
         <v>44360</v>
       </c>
       <c r="B746" t="n">
-        <v>117.7333333333333</v>
+        <v>117.9</v>
       </c>
     </row>
     <row r="747">
@@ -6414,7 +6414,7 @@
         <v>44361</v>
       </c>
       <c r="B747" t="n">
-        <v>117.8666666666667</v>
+        <v>118.075</v>
       </c>
     </row>
     <row r="748">
@@ -6422,7 +6422,7 @@
         <v>44362</v>
       </c>
       <c r="B748" t="n">
-        <v>118</v>
+        <v>118.25</v>
       </c>
     </row>
     <row r="749">
@@ -6430,7 +6430,7 @@
         <v>44363</v>
       </c>
       <c r="B749" t="n">
-        <v>118.1333333333333</v>
+        <v>118.425</v>
       </c>
     </row>
     <row r="750">
@@ -6438,7 +6438,7 @@
         <v>44364</v>
       </c>
       <c r="B750" t="n">
-        <v>118.2666666666667</v>
+        <v>118.6</v>
       </c>
     </row>
     <row r="751">
@@ -6846,7 +6846,7 @@
         <v>44415</v>
       </c>
       <c r="B801" t="n">
-        <v>99.53333333333333</v>
+        <v>99.53333333333335</v>
       </c>
     </row>
     <row r="802">
@@ -7182,7 +7182,7 @@
         <v>44457</v>
       </c>
       <c r="B843" t="n">
-        <v>97.69999999999999</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="844">
@@ -7518,7 +7518,7 @@
         <v>44499</v>
       </c>
       <c r="B885" t="n">
-        <v>127.7705882352941</v>
+        <v>128.8666666666667</v>
       </c>
     </row>
     <row r="886">
@@ -7526,7 +7526,7 @@
         <v>44500</v>
       </c>
       <c r="B886" t="n">
-        <v>127.7411764705882</v>
+        <v>129.9333333333333</v>
       </c>
     </row>
     <row r="887">
@@ -7534,7 +7534,7 @@
         <v>44501</v>
       </c>
       <c r="B887" t="n">
-        <v>127.7117647058823</v>
+        <v>131</v>
       </c>
     </row>
     <row r="888">
@@ -7542,7 +7542,7 @@
         <v>44502</v>
       </c>
       <c r="B888" t="n">
-        <v>127.6823529411765</v>
+        <v>131</v>
       </c>
     </row>
     <row r="889">
@@ -7550,7 +7550,7 @@
         <v>44503</v>
       </c>
       <c r="B889" t="n">
-        <v>127.6529411764706</v>
+        <v>134.2</v>
       </c>
     </row>
     <row r="890">
@@ -7558,7 +7558,7 @@
         <v>44504</v>
       </c>
       <c r="B890" t="n">
-        <v>127.6235294117647</v>
+        <v>132.1</v>
       </c>
     </row>
     <row r="891">
@@ -7566,7 +7566,7 @@
         <v>44505</v>
       </c>
       <c r="B891" t="n">
-        <v>127.5941176470588</v>
+        <v>130</v>
       </c>
     </row>
     <row r="892">
@@ -7574,7 +7574,7 @@
         <v>44506</v>
       </c>
       <c r="B892" t="n">
-        <v>127.5647058823529</v>
+        <v>87.52799999999999</v>
       </c>
     </row>
     <row r="893">
@@ -7582,7 +7582,7 @@
         <v>44507</v>
       </c>
       <c r="B893" t="n">
-        <v>127.5352941176471</v>
+        <v>45.056</v>
       </c>
     </row>
     <row r="894">
@@ -7590,7 +7590,7 @@
         <v>44508</v>
       </c>
       <c r="B894" t="n">
-        <v>127.5058823529412</v>
+        <v>129.2</v>
       </c>
     </row>
     <row r="895">
@@ -7598,7 +7598,7 @@
         <v>44509</v>
       </c>
       <c r="B895" t="n">
-        <v>127.4764705882353</v>
+        <v>127</v>
       </c>
     </row>
     <row r="896">
@@ -7606,7 +7606,7 @@
         <v>44510</v>
       </c>
       <c r="B896" t="n">
-        <v>127.4470588235294</v>
+        <v>127.4</v>
       </c>
     </row>
     <row r="897">
@@ -7614,7 +7614,7 @@
         <v>44511</v>
       </c>
       <c r="B897" t="n">
-        <v>127.4176470588235</v>
+        <v>128.6</v>
       </c>
     </row>
     <row r="898">
@@ -7622,7 +7622,7 @@
         <v>44512</v>
       </c>
       <c r="B898" t="n">
-        <v>127.3882352941176</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="899">
@@ -7630,7 +7630,7 @@
         <v>44513</v>
       </c>
       <c r="B899" t="n">
-        <v>127.3588235294118</v>
+        <v>126.6</v>
       </c>
     </row>
     <row r="900">
@@ -7638,7 +7638,7 @@
         <v>44514</v>
       </c>
       <c r="B900" t="n">
-        <v>127.3294117647059</v>
+        <v>126.4</v>
       </c>
     </row>
     <row r="901">
@@ -7646,7 +7646,7 @@
         <v>44515</v>
       </c>
       <c r="B901" t="n">
-        <v>127.3</v>
+        <v>126.2</v>
       </c>
     </row>
     <row r="902">
@@ -7654,7 +7654,7 @@
         <v>44516</v>
       </c>
       <c r="B902" t="n">
-        <v>127.2705882352941</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="903">
@@ -7662,7 +7662,7 @@
         <v>44517</v>
       </c>
       <c r="B903" t="n">
-        <v>127.2411764705882</v>
+        <v>123.2</v>
       </c>
     </row>
     <row r="904">
@@ -7670,7 +7670,7 @@
         <v>44518</v>
       </c>
       <c r="B904" t="n">
-        <v>127.2117647058823</v>
+        <v>124.4</v>
       </c>
     </row>
     <row r="905">
@@ -7678,7 +7678,7 @@
         <v>44519</v>
       </c>
       <c r="B905" t="n">
-        <v>127.1823529411765</v>
+        <v>125.6</v>
       </c>
     </row>
     <row r="906">
@@ -7686,7 +7686,7 @@
         <v>44520</v>
       </c>
       <c r="B906" t="n">
-        <v>127.1529411764706</v>
+        <v>125.55</v>
       </c>
     </row>
     <row r="907">
@@ -7694,7 +7694,7 @@
         <v>44521</v>
       </c>
       <c r="B907" t="n">
-        <v>127.1235294117647</v>
+        <v>125.5</v>
       </c>
     </row>
     <row r="908">
@@ -7702,7 +7702,7 @@
         <v>44522</v>
       </c>
       <c r="B908" t="n">
-        <v>127.0941176470588</v>
+        <v>125.45</v>
       </c>
     </row>
     <row r="909">
@@ -7710,7 +7710,7 @@
         <v>44523</v>
       </c>
       <c r="B909" t="n">
-        <v>127.0647058823529</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="910">
@@ -7718,7 +7718,7 @@
         <v>44524</v>
       </c>
       <c r="B910" t="n">
-        <v>127.0352941176471</v>
+        <v>126</v>
       </c>
     </row>
     <row r="911">
@@ -7726,7 +7726,7 @@
         <v>44525</v>
       </c>
       <c r="B911" t="n">
-        <v>127.0058823529412</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="912">
@@ -7734,7 +7734,7 @@
         <v>44526</v>
       </c>
       <c r="B912" t="n">
-        <v>126.9764705882353</v>
+        <v>125.2</v>
       </c>
     </row>
     <row r="913">
@@ -7742,7 +7742,7 @@
         <v>44527</v>
       </c>
       <c r="B913" t="n">
-        <v>126.9470588235294</v>
+        <v>125.7333333333333</v>
       </c>
     </row>
     <row r="914">
@@ -7750,7 +7750,7 @@
         <v>44528</v>
       </c>
       <c r="B914" t="n">
-        <v>126.9176470588235</v>
+        <v>126.2666666666667</v>
       </c>
     </row>
     <row r="915">
@@ -7758,7 +7758,7 @@
         <v>44529</v>
       </c>
       <c r="B915" t="n">
-        <v>126.8882352941176</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="916">
@@ -7766,7 +7766,7 @@
         <v>44530</v>
       </c>
       <c r="B916" t="n">
-        <v>126.8588235294118</v>
+        <v>126.4</v>
       </c>
     </row>
     <row r="917">
@@ -7774,7 +7774,7 @@
         <v>44531</v>
       </c>
       <c r="B917" t="n">
-        <v>126.8294117647059</v>
+        <v>126.2</v>
       </c>
     </row>
     <row r="918">
@@ -12758,7 +12758,7 @@
         <v>45154</v>
       </c>
       <c r="B1540" t="n">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="1541">
@@ -15071,6 +15071,1326 @@
       </c>
       <c r="B1829" t="n">
         <v>205.5</v>
+      </c>
+    </row>
+    <row r="1830">
+      <c r="A1830" s="2" t="n">
+        <v>45444</v>
+      </c>
+      <c r="B1830" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1831">
+      <c r="A1831" s="2" t="n">
+        <v>45445</v>
+      </c>
+      <c r="B1831" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1832">
+      <c r="A1832" s="2" t="n">
+        <v>45446</v>
+      </c>
+      <c r="B1832" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1833">
+      <c r="A1833" s="2" t="n">
+        <v>45447</v>
+      </c>
+      <c r="B1833" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1834">
+      <c r="A1834" s="2" t="n">
+        <v>45448</v>
+      </c>
+      <c r="B1834" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1835">
+      <c r="A1835" s="2" t="n">
+        <v>45449</v>
+      </c>
+      <c r="B1835" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" s="2" t="n">
+        <v>45450</v>
+      </c>
+      <c r="B1836" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1837">
+      <c r="A1837" s="2" t="n">
+        <v>45451</v>
+      </c>
+      <c r="B1837" t="n">
+        <v>205.8333333333333</v>
+      </c>
+    </row>
+    <row r="1838">
+      <c r="A1838" s="2" t="n">
+        <v>45452</v>
+      </c>
+      <c r="B1838" t="n">
+        <v>205.6666666666667</v>
+      </c>
+    </row>
+    <row r="1839">
+      <c r="A1839" s="2" t="n">
+        <v>45453</v>
+      </c>
+      <c r="B1839" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1840">
+      <c r="A1840" s="2" t="n">
+        <v>45454</v>
+      </c>
+      <c r="B1840" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1841">
+      <c r="A1841" s="2" t="n">
+        <v>45455</v>
+      </c>
+      <c r="B1841" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" s="2" t="n">
+        <v>45456</v>
+      </c>
+      <c r="B1842" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" s="2" t="n">
+        <v>45457</v>
+      </c>
+      <c r="B1843" t="n">
+        <v>205.4</v>
+      </c>
+    </row>
+    <row r="1844">
+      <c r="A1844" s="2" t="n">
+        <v>45458</v>
+      </c>
+      <c r="B1844" t="n">
+        <v>205.4675</v>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" s="2" t="n">
+        <v>45459</v>
+      </c>
+      <c r="B1845" t="n">
+        <v>205.535</v>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" s="2" t="n">
+        <v>45460</v>
+      </c>
+      <c r="B1846" t="n">
+        <v>205.6025</v>
+      </c>
+    </row>
+    <row r="1847">
+      <c r="A1847" s="2" t="n">
+        <v>45461</v>
+      </c>
+      <c r="B1847" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" s="2" t="n">
+        <v>45462</v>
+      </c>
+      <c r="B1848" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" s="2" t="n">
+        <v>45463</v>
+      </c>
+      <c r="B1849" t="n">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="1850">
+      <c r="A1850" s="2" t="n">
+        <v>45464</v>
+      </c>
+      <c r="B1850" t="n">
+        <v>206.105</v>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" s="2" t="n">
+        <v>45465</v>
+      </c>
+      <c r="B1851" t="n">
+        <v>205.96</v>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" s="2" t="n">
+        <v>45466</v>
+      </c>
+      <c r="B1852" t="n">
+        <v>205.815</v>
+      </c>
+    </row>
+    <row r="1853">
+      <c r="A1853" s="2" t="n">
+        <v>45467</v>
+      </c>
+      <c r="B1853" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" s="2" t="n">
+        <v>45468</v>
+      </c>
+      <c r="B1854" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" s="2" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1855" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1856">
+      <c r="A1856" s="2" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1856" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" s="2" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1857" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" s="2" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1858" t="n">
+        <v>205.6133333333333</v>
+      </c>
+    </row>
+    <row r="1859">
+      <c r="A1859" s="2" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1859" t="n">
+        <v>205.5566666666667</v>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" s="2" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1860" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" s="2" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1861" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1862">
+      <c r="A1862" s="2" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1862" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" s="2" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1863" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" s="2" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1864" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1865">
+      <c r="A1865" s="2" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1865" t="n">
+        <v>205.78</v>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" s="2" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1866" t="n">
+        <v>205.89</v>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" s="2" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1867" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1868">
+      <c r="A1868" s="2" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1868" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1869">
+      <c r="A1869" s="2" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1869" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" s="2" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1870" t="n">
+        <v>206.5</v>
+      </c>
+    </row>
+    <row r="1871">
+      <c r="A1871" s="2" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1871" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" s="2" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1872" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" s="2" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1873" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1874">
+      <c r="A1874" s="2" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1874" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1875">
+      <c r="A1875" s="2" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1875" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="1876">
+      <c r="A1876" s="2" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1876" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" s="2" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1877" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" s="2" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1878" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" s="2" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1879" t="n">
+        <v>205.4433333333333</v>
+      </c>
+    </row>
+    <row r="1880">
+      <c r="A1880" s="2" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1880" t="n">
+        <v>205.8866666666667</v>
+      </c>
+    </row>
+    <row r="1881">
+      <c r="A1881" s="2" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1881" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1882">
+      <c r="A1882" s="2" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1882" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1883">
+      <c r="A1883" s="2" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1883" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1884">
+      <c r="A1884" s="2" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1884" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1885">
+      <c r="A1885" s="2" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1885" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1886">
+      <c r="A1886" s="2" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1886" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1887">
+      <c r="A1887" s="2" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1887" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1888">
+      <c r="A1888" s="2" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1888" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1889">
+      <c r="A1889" s="2" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1889" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1890">
+      <c r="A1890" s="2" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1890" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1891">
+      <c r="A1891" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1891" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1892">
+      <c r="A1892" s="2" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1892" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1893">
+      <c r="A1893" s="2" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1893" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1894">
+      <c r="A1894" s="2" t="n">
+        <v>45508</v>
+      </c>
+      <c r="B1894" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1895">
+      <c r="A1895" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="B1895" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1896">
+      <c r="A1896" s="2" t="n">
+        <v>45510</v>
+      </c>
+      <c r="B1896" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1897">
+      <c r="A1897" s="2" t="n">
+        <v>45511</v>
+      </c>
+      <c r="B1897" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1898">
+      <c r="A1898" s="2" t="n">
+        <v>45512</v>
+      </c>
+      <c r="B1898" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1899">
+      <c r="A1899" s="2" t="n">
+        <v>45513</v>
+      </c>
+      <c r="B1899" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1900">
+      <c r="A1900" s="2" t="n">
+        <v>45514</v>
+      </c>
+      <c r="B1900" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1901">
+      <c r="A1901" s="2" t="n">
+        <v>45515</v>
+      </c>
+      <c r="B1901" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1902">
+      <c r="A1902" s="2" t="n">
+        <v>45516</v>
+      </c>
+      <c r="B1902" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1903">
+      <c r="A1903" s="2" t="n">
+        <v>45517</v>
+      </c>
+      <c r="B1903" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1904">
+      <c r="A1904" s="2" t="n">
+        <v>45518</v>
+      </c>
+      <c r="B1904" t="n">
+        <v>205.67</v>
+      </c>
+    </row>
+    <row r="1905">
+      <c r="A1905" s="2" t="n">
+        <v>45519</v>
+      </c>
+      <c r="B1905" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1906">
+      <c r="A1906" s="2" t="n">
+        <v>45520</v>
+      </c>
+      <c r="B1906" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1907">
+      <c r="A1907" s="2" t="n">
+        <v>45521</v>
+      </c>
+      <c r="B1907" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1908">
+      <c r="A1908" s="2" t="n">
+        <v>45522</v>
+      </c>
+      <c r="B1908" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1909">
+      <c r="A1909" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="B1909" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1910">
+      <c r="A1910" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="B1910" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1911">
+      <c r="A1911" s="2" t="n">
+        <v>45525</v>
+      </c>
+      <c r="B1911" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1912">
+      <c r="A1912" s="2" t="n">
+        <v>45526</v>
+      </c>
+      <c r="B1912" t="n">
+        <v>206.33</v>
+      </c>
+    </row>
+    <row r="1913">
+      <c r="A1913" s="2" t="n">
+        <v>45527</v>
+      </c>
+      <c r="B1913" t="n">
+        <v>207.33</v>
+      </c>
+    </row>
+    <row r="1914">
+      <c r="A1914" s="2" t="n">
+        <v>45528</v>
+      </c>
+      <c r="B1914" t="n">
+        <v>207.8866666666667</v>
+      </c>
+    </row>
+    <row r="1915">
+      <c r="A1915" s="2" t="n">
+        <v>45529</v>
+      </c>
+      <c r="B1915" t="n">
+        <v>208.4433333333333</v>
+      </c>
+    </row>
+    <row r="1916">
+      <c r="A1916" s="2" t="n">
+        <v>45530</v>
+      </c>
+      <c r="B1916" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1917">
+      <c r="A1917" s="2" t="n">
+        <v>45531</v>
+      </c>
+      <c r="B1917" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1918">
+      <c r="A1918" s="2" t="n">
+        <v>45532</v>
+      </c>
+      <c r="B1918" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1919">
+      <c r="A1919" s="2" t="n">
+        <v>45533</v>
+      </c>
+      <c r="B1919" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1920">
+      <c r="A1920" s="2" t="n">
+        <v>45534</v>
+      </c>
+      <c r="B1920" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1921">
+      <c r="A1921" s="2" t="n">
+        <v>45535</v>
+      </c>
+      <c r="B1921" t="n">
+        <v>209.6666666666667</v>
+      </c>
+    </row>
+    <row r="1922">
+      <c r="A1922" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B1922" t="n">
+        <v>210.3333333333333</v>
+      </c>
+    </row>
+    <row r="1923">
+      <c r="A1923" s="2" t="n">
+        <v>45537</v>
+      </c>
+      <c r="B1923" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1924">
+      <c r="A1924" s="2" t="n">
+        <v>45538</v>
+      </c>
+      <c r="B1924" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1925">
+      <c r="A1925" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="B1925" t="n">
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="1926">
+      <c r="A1926" s="2" t="n">
+        <v>45540</v>
+      </c>
+      <c r="B1926" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1927">
+      <c r="A1927" s="2" t="n">
+        <v>45541</v>
+      </c>
+      <c r="B1927" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1928">
+      <c r="A1928" s="2" t="n">
+        <v>45542</v>
+      </c>
+      <c r="B1928" t="n">
+        <v>212.6666666666667</v>
+      </c>
+    </row>
+    <row r="1929">
+      <c r="A1929" s="2" t="n">
+        <v>45543</v>
+      </c>
+      <c r="B1929" t="n">
+        <v>214.3333333333333</v>
+      </c>
+    </row>
+    <row r="1930">
+      <c r="A1930" s="2" t="n">
+        <v>45544</v>
+      </c>
+      <c r="B1930" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1931">
+      <c r="A1931" s="2" t="n">
+        <v>45545</v>
+      </c>
+      <c r="B1931" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1932">
+      <c r="A1932" s="2" t="n">
+        <v>45546</v>
+      </c>
+      <c r="B1932" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1933">
+      <c r="A1933" s="2" t="n">
+        <v>45547</v>
+      </c>
+      <c r="B1933" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1934">
+      <c r="A1934" s="2" t="n">
+        <v>45548</v>
+      </c>
+      <c r="B1934" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1935">
+      <c r="A1935" s="2" t="n">
+        <v>45549</v>
+      </c>
+      <c r="B1935" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1936">
+      <c r="A1936" s="2" t="n">
+        <v>45550</v>
+      </c>
+      <c r="B1936" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1937">
+      <c r="A1937" s="2" t="n">
+        <v>45551</v>
+      </c>
+      <c r="B1937" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1938">
+      <c r="A1938" s="2" t="n">
+        <v>45552</v>
+      </c>
+      <c r="B1938" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1939">
+      <c r="A1939" s="2" t="n">
+        <v>45553</v>
+      </c>
+      <c r="B1939" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1940">
+      <c r="A1940" s="2" t="n">
+        <v>45554</v>
+      </c>
+      <c r="B1940" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1941">
+      <c r="A1941" s="2" t="n">
+        <v>45555</v>
+      </c>
+      <c r="B1941" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1942">
+      <c r="A1942" s="2" t="n">
+        <v>45556</v>
+      </c>
+      <c r="B1942" t="n">
+        <v>216.875</v>
+      </c>
+    </row>
+    <row r="1943">
+      <c r="A1943" s="2" t="n">
+        <v>45557</v>
+      </c>
+      <c r="B1943" t="n">
+        <v>217.75</v>
+      </c>
+    </row>
+    <row r="1944">
+      <c r="A1944" s="2" t="n">
+        <v>45558</v>
+      </c>
+      <c r="B1944" t="n">
+        <v>218.625</v>
+      </c>
+    </row>
+    <row r="1945">
+      <c r="A1945" s="2" t="n">
+        <v>45559</v>
+      </c>
+      <c r="B1945" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1946">
+      <c r="A1946" s="2" t="n">
+        <v>45560</v>
+      </c>
+      <c r="B1946" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1947">
+      <c r="A1947" s="2" t="n">
+        <v>45561</v>
+      </c>
+      <c r="B1947" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1948">
+      <c r="A1948" s="2" t="n">
+        <v>45562</v>
+      </c>
+      <c r="B1948" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1949">
+      <c r="A1949" s="2" t="n">
+        <v>45563</v>
+      </c>
+      <c r="B1949" t="n">
+        <v>218.5</v>
+      </c>
+    </row>
+    <row r="1950">
+      <c r="A1950" s="2" t="n">
+        <v>45564</v>
+      </c>
+      <c r="B1950" t="n">
+        <v>217.5</v>
+      </c>
+    </row>
+    <row r="1951">
+      <c r="A1951" s="2" t="n">
+        <v>45565</v>
+      </c>
+      <c r="B1951" t="n">
+        <v>216.5</v>
+      </c>
+    </row>
+    <row r="1952">
+      <c r="A1952" s="2" t="n">
+        <v>45566</v>
+      </c>
+      <c r="B1952" t="n">
+        <v>216.5</v>
+      </c>
+    </row>
+    <row r="1953">
+      <c r="A1953" s="2" t="n">
+        <v>45567</v>
+      </c>
+      <c r="B1953" t="n">
+        <v>216.5</v>
+      </c>
+    </row>
+    <row r="1954">
+      <c r="A1954" s="2" t="n">
+        <v>45568</v>
+      </c>
+      <c r="B1954" t="n">
+        <v>214.25</v>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" s="2" t="n">
+        <v>45569</v>
+      </c>
+      <c r="B1955" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="1956">
+      <c r="A1956" s="2" t="n">
+        <v>45570</v>
+      </c>
+      <c r="B1956" t="n">
+        <v>214.6666666666667</v>
+      </c>
+    </row>
+    <row r="1957">
+      <c r="A1957" s="2" t="n">
+        <v>45571</v>
+      </c>
+      <c r="B1957" t="n">
+        <v>214.3333333333333</v>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" s="2" t="n">
+        <v>45572</v>
+      </c>
+      <c r="B1958" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" s="2" t="n">
+        <v>45573</v>
+      </c>
+      <c r="B1959" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" s="2" t="n">
+        <v>45574</v>
+      </c>
+      <c r="B1960" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1961">
+      <c r="A1961" s="2" t="n">
+        <v>45575</v>
+      </c>
+      <c r="B1961" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1962">
+      <c r="A1962" s="2" t="n">
+        <v>45576</v>
+      </c>
+      <c r="B1962" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1963">
+      <c r="A1963" s="2" t="n">
+        <v>45577</v>
+      </c>
+      <c r="B1963" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1964">
+      <c r="A1964" s="2" t="n">
+        <v>45578</v>
+      </c>
+      <c r="B1964" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1965">
+      <c r="A1965" s="2" t="n">
+        <v>45579</v>
+      </c>
+      <c r="B1965" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="1966">
+      <c r="A1966" s="2" t="n">
+        <v>45580</v>
+      </c>
+      <c r="B1966" t="n">
+        <v>214.33</v>
+      </c>
+    </row>
+    <row r="1967">
+      <c r="A1967" s="2" t="n">
+        <v>45581</v>
+      </c>
+      <c r="B1967" t="n">
+        <v>214.5</v>
+      </c>
+    </row>
+    <row r="1968">
+      <c r="A1968" s="2" t="n">
+        <v>45582</v>
+      </c>
+      <c r="B1968" t="n">
+        <v>215.75</v>
+      </c>
+    </row>
+    <row r="1969">
+      <c r="A1969" s="2" t="n">
+        <v>45583</v>
+      </c>
+      <c r="B1969" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1970">
+      <c r="A1970" s="2" t="n">
+        <v>45584</v>
+      </c>
+      <c r="B1970" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1971">
+      <c r="A1971" s="2" t="n">
+        <v>45585</v>
+      </c>
+      <c r="B1971" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1972">
+      <c r="A1972" s="2" t="n">
+        <v>45586</v>
+      </c>
+      <c r="B1972" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1973">
+      <c r="A1973" s="2" t="n">
+        <v>45587</v>
+      </c>
+      <c r="B1973" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1974">
+      <c r="A1974" s="2" t="n">
+        <v>45588</v>
+      </c>
+      <c r="B1974" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1975">
+      <c r="A1975" s="2" t="n">
+        <v>45589</v>
+      </c>
+      <c r="B1975" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1976">
+      <c r="A1976" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="B1976" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1977">
+      <c r="A1977" s="2" t="n">
+        <v>45591</v>
+      </c>
+      <c r="B1977" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1978">
+      <c r="A1978" s="2" t="n">
+        <v>45592</v>
+      </c>
+      <c r="B1978" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1979">
+      <c r="A1979" s="2" t="n">
+        <v>45593</v>
+      </c>
+      <c r="B1979" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1980">
+      <c r="A1980" s="2" t="n">
+        <v>45594</v>
+      </c>
+      <c r="B1980" t="n">
+        <v>219.2</v>
+      </c>
+    </row>
+    <row r="1981">
+      <c r="A1981" s="2" t="n">
+        <v>45595</v>
+      </c>
+      <c r="B1981" t="n">
+        <v>219.3</v>
+      </c>
+    </row>
+    <row r="1982">
+      <c r="A1982" s="2" t="n">
+        <v>45596</v>
+      </c>
+      <c r="B1982" t="n">
+        <v>219.4</v>
+      </c>
+    </row>
+    <row r="1983">
+      <c r="A1983" s="2" t="n">
+        <v>45597</v>
+      </c>
+      <c r="B1983" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1984">
+      <c r="A1984" s="2" t="n">
+        <v>45598</v>
+      </c>
+      <c r="B1984" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" s="2" t="n">
+        <v>45599</v>
+      </c>
+      <c r="B1985" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1986">
+      <c r="A1986" s="2" t="n">
+        <v>45600</v>
+      </c>
+      <c r="B1986" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1987">
+      <c r="A1987" s="2" t="n">
+        <v>45601</v>
+      </c>
+      <c r="B1987" t="n">
+        <v>219.33</v>
+      </c>
+    </row>
+    <row r="1988">
+      <c r="A1988" s="2" t="n">
+        <v>45602</v>
+      </c>
+      <c r="B1988" t="n">
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="1989">
+      <c r="A1989" s="2" t="n">
+        <v>45603</v>
+      </c>
+      <c r="B1989" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="1990">
+      <c r="A1990" s="2" t="n">
+        <v>45604</v>
+      </c>
+      <c r="B1990" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="1991">
+      <c r="A1991" s="2" t="n">
+        <v>45605</v>
+      </c>
+      <c r="B1991" t="n">
+        <v>219.0825</v>
+      </c>
+    </row>
+    <row r="1992">
+      <c r="A1992" s="2" t="n">
+        <v>45606</v>
+      </c>
+      <c r="B1992" t="n">
+        <v>219.165</v>
+      </c>
+    </row>
+    <row r="1993">
+      <c r="A1993" s="2" t="n">
+        <v>45607</v>
+      </c>
+      <c r="B1993" t="n">
+        <v>219.2475</v>
+      </c>
+    </row>
+    <row r="1994">
+      <c r="A1994" s="2" t="n">
+        <v>45608</v>
+      </c>
+      <c r="B1994" t="n">
+        <v>219.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>